<commit_message>
Sync site with AppSumo tracker: add New apps, remove Delete apps
- Add 12 New apps: Kavout, MyClone, Unmixr AI, DREAMLIT, Airbrush, WPAutoBlog, Tiny Talk, PISMO, WebAbility.io, Fynlo, personeo.ai, XInterview AI
- Add to reviews.html, create tool review pages, best-lifetime-ai-tools, sitemap
- Remove 31 Delete apps from site: delete tool pages, compare pages (beehiiv vs substack, systeme vs clickfunnels), remove from reviews, guides, category, best, sitemap
- Update guides to replace deleted app mentions (e.g. Beehiiv -> SendFox/MailerLite)
</commit_message>
<xml_diff>
--- a/appsumo-affiliate-links-tracker.xlsx
+++ b/appsumo-affiliate-links-tracker.xlsx
@@ -13,17 +13,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1768962967" val="1068" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1768962967" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1768962967" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1768962967"/>
+      <pm:revision xmlns:pm="smNativeData" day="1769222744" val="1068" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1769222744" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1769222744" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1769222744"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="357">
   <si>
     <t>Product Name</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Triplo AI</t>
   </si>
   <si>
@@ -55,7 +52,7 @@
     <t>https://appsumo.8odi.net/9L4b7e</t>
   </si>
   <si>
-    <t>Pending</t>
+    <t>Unavailable</t>
   </si>
   <si>
     <t>ClickRank</t>
@@ -70,6 +67,9 @@
     <t>https://appsumo.8odi.net/rakAmG</t>
   </si>
   <si>
+    <t>Active</t>
+  </si>
+  <si>
     <t>TidyCal</t>
   </si>
   <si>
@@ -82,9 +82,6 @@
     <t>https://appsumo.8odi.net/jexM9n</t>
   </si>
   <si>
-    <t>Example: appsumo.8odi.net/9L4boe</t>
-  </si>
-  <si>
     <t>NeuronWriter</t>
   </si>
   <si>
@@ -181,6 +178,9 @@
     <t>https://appsumo.8odi.net/2abGZG</t>
   </si>
   <si>
+    <t>Delete</t>
+  </si>
+  <si>
     <t>Robinize</t>
   </si>
   <si>
@@ -947,6 +947,153 @@
   </si>
   <si>
     <t>https://appsumo.8odi.net/Xm0QDG</t>
+  </si>
+  <si>
+    <t>Kavout</t>
+  </si>
+  <si>
+    <t>kavout</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/kavout/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/MAa2rP</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>MyClone</t>
+  </si>
+  <si>
+    <t>myclone</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/myclone/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/mOxjQD</t>
+  </si>
+  <si>
+    <t>Unmixr AI</t>
+  </si>
+  <si>
+    <t>unmixr-ai</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/unmixr-ai/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/PO1RP6</t>
+  </si>
+  <si>
+    <t>DREAMLIT</t>
+  </si>
+  <si>
+    <t>dreamlit-ai</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/dreamlit-ai/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/PO1RPq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Airbrush </t>
+  </si>
+  <si>
+    <t>airbrush-ai-image-generator</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/airbrush-ai-image-generator/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/XmzGVM</t>
+  </si>
+  <si>
+    <t>WPAutoBlog</t>
+  </si>
+  <si>
+    <t>wpautoblogcom</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/wpautoblogcom/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/090yeL</t>
+  </si>
+  <si>
+    <t>Tiny Talk</t>
+  </si>
+  <si>
+    <t>tiny-talk</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/tiny-talk/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/2anyAG</t>
+  </si>
+  <si>
+    <t>PISMO</t>
+  </si>
+  <si>
+    <t>pismo-alt</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/pismo-alt/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/dO4kQy</t>
+  </si>
+  <si>
+    <t>WebAbility.io</t>
+  </si>
+  <si>
+    <t>webabilityio</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/webabilityio/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/yqGj0y</t>
+  </si>
+  <si>
+    <t>Fynlo</t>
+  </si>
+  <si>
+    <t>fynlo</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/fynlo/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/YRWb6q</t>
+  </si>
+  <si>
+    <t>personeo.ai</t>
+  </si>
+  <si>
+    <t>personeoai</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/personeoai/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/K0kO1z</t>
+  </si>
+  <si>
+    <t>XInterview AI</t>
+  </si>
+  <si>
+    <t>xinterview</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/xinterview/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/7a3n2O</t>
   </si>
 </sst>
 </file>
@@ -971,7 +1118,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1768962967" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1769222744" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -993,7 +1140,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1768962967" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1769222744" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1015,7 +1162,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1768962967"/>
+          <pm:border xmlns:pm="smNativeData" id="1769222744"/>
         </ext>
       </extLst>
     </border>
@@ -1034,7 +1181,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1768962967"/>
+          <pm:border xmlns:pm="smNativeData" id="1769222744"/>
         </ext>
       </extLst>
     </border>
@@ -1051,7 +1198,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1768962967" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1769222744" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -1315,10 +1462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:F76"/>
+  <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -1327,7 +1474,7 @@
     <col min="2" max="2" width="19.081081" customWidth="1" style="0"/>
     <col min="3" max="3" width="48.918919" customWidth="1" style="0"/>
     <col min="4" max="4" width="42.756757" customWidth="1" style="0"/>
-    <col min="5" max="6" width="10.000000" style="0"/>
+    <col min="5" max="5" width="10.000000" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1346,42 +1493,39 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1398,146 +1542,143 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>26</v>
       </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>29</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>30</v>
       </c>
-      <c r="D7" t="s">
-        <v>31</v>
-      </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>34</v>
       </c>
-      <c r="D8" t="s">
-        <v>35</v>
-      </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
         <v>36</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>37</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>38</v>
       </c>
-      <c r="D9" t="s">
-        <v>39</v>
-      </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
         <v>40</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>41</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>42</v>
       </c>
-      <c r="D10" t="s">
-        <v>43</v>
-      </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s">
         <v>44</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>45</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>46</v>
       </c>
-      <c r="D11" t="s">
-        <v>47</v>
-      </c>
       <c r="E11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
         <v>48</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>49</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>50</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>51</v>
-      </c>
-      <c r="E12" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1554,7 +1695,7 @@
         <v>55</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1571,7 +1712,7 @@
         <v>59</v>
       </c>
       <c r="E14" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1588,7 +1729,7 @@
         <v>63</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1605,7 +1746,7 @@
         <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1622,7 +1763,7 @@
         <v>71</v>
       </c>
       <c r="E17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1639,7 +1780,7 @@
         <v>75</v>
       </c>
       <c r="E18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1656,7 +1797,7 @@
         <v>79</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1673,7 +1814,7 @@
         <v>83</v>
       </c>
       <c r="E20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1690,7 +1831,7 @@
         <v>87</v>
       </c>
       <c r="E21" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1707,7 +1848,7 @@
         <v>91</v>
       </c>
       <c r="E22" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1724,7 +1865,7 @@
         <v>95</v>
       </c>
       <c r="E23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1741,7 +1882,7 @@
         <v>99</v>
       </c>
       <c r="E24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1758,7 +1899,7 @@
         <v>103</v>
       </c>
       <c r="E25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1775,7 +1916,7 @@
         <v>107</v>
       </c>
       <c r="E26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1792,7 +1933,7 @@
         <v>111</v>
       </c>
       <c r="E27" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1809,7 +1950,7 @@
         <v>115</v>
       </c>
       <c r="E28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1826,7 +1967,7 @@
         <v>119</v>
       </c>
       <c r="E29" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1843,7 +1984,7 @@
         <v>123</v>
       </c>
       <c r="E30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1860,7 +2001,7 @@
         <v>127</v>
       </c>
       <c r="E31" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1877,7 +2018,7 @@
         <v>131</v>
       </c>
       <c r="E32" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1894,7 +2035,7 @@
         <v>135</v>
       </c>
       <c r="E33" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1911,7 +2052,7 @@
         <v>139</v>
       </c>
       <c r="E34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1928,7 +2069,7 @@
         <v>143</v>
       </c>
       <c r="E35" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1945,7 +2086,7 @@
         <v>147</v>
       </c>
       <c r="E36" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1962,7 +2103,7 @@
         <v>151</v>
       </c>
       <c r="E37" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1979,7 +2120,7 @@
         <v>155</v>
       </c>
       <c r="E38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1996,7 +2137,7 @@
         <v>159</v>
       </c>
       <c r="E39" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -2013,7 +2154,7 @@
         <v>163</v>
       </c>
       <c r="E40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -2030,7 +2171,7 @@
         <v>167</v>
       </c>
       <c r="E41" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -2047,7 +2188,7 @@
         <v>171</v>
       </c>
       <c r="E42" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -2064,7 +2205,7 @@
         <v>175</v>
       </c>
       <c r="E43" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -2081,7 +2222,7 @@
         <v>179</v>
       </c>
       <c r="E44" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -2098,7 +2239,7 @@
         <v>183</v>
       </c>
       <c r="E45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -2115,7 +2256,7 @@
         <v>187</v>
       </c>
       <c r="E46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -2132,7 +2273,7 @@
         <v>191</v>
       </c>
       <c r="E47" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -2149,7 +2290,7 @@
         <v>195</v>
       </c>
       <c r="E48" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -2166,7 +2307,7 @@
         <v>199</v>
       </c>
       <c r="E49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -2183,7 +2324,7 @@
         <v>203</v>
       </c>
       <c r="E50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -2200,7 +2341,7 @@
         <v>207</v>
       </c>
       <c r="E51" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2217,7 +2358,7 @@
         <v>211</v>
       </c>
       <c r="E52" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -2234,7 +2375,7 @@
         <v>215</v>
       </c>
       <c r="E53" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2251,7 +2392,7 @@
         <v>219</v>
       </c>
       <c r="E54" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -2268,7 +2409,7 @@
         <v>223</v>
       </c>
       <c r="E55" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2285,7 +2426,7 @@
         <v>227</v>
       </c>
       <c r="E56" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -2302,7 +2443,7 @@
         <v>231</v>
       </c>
       <c r="E57" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2319,7 +2460,7 @@
         <v>235</v>
       </c>
       <c r="E58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -2336,7 +2477,7 @@
         <v>239</v>
       </c>
       <c r="E59" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -2353,7 +2494,7 @@
         <v>243</v>
       </c>
       <c r="E60" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -2370,7 +2511,7 @@
         <v>247</v>
       </c>
       <c r="E61" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -2387,7 +2528,7 @@
         <v>251</v>
       </c>
       <c r="E62" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -2404,7 +2545,7 @@
         <v>255</v>
       </c>
       <c r="E63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -2421,7 +2562,7 @@
         <v>259</v>
       </c>
       <c r="E64" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -2438,7 +2579,7 @@
         <v>263</v>
       </c>
       <c r="E65" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -2455,7 +2596,7 @@
         <v>267</v>
       </c>
       <c r="E66" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -2472,7 +2613,7 @@
         <v>271</v>
       </c>
       <c r="E67" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -2489,7 +2630,7 @@
         <v>275</v>
       </c>
       <c r="E68" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -2506,7 +2647,7 @@
         <v>279</v>
       </c>
       <c r="E69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -2523,7 +2664,7 @@
         <v>283</v>
       </c>
       <c r="E70" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2540,7 +2681,7 @@
         <v>287</v>
       </c>
       <c r="E71" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -2557,7 +2698,7 @@
         <v>291</v>
       </c>
       <c r="E72" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -2574,7 +2715,7 @@
         <v>295</v>
       </c>
       <c r="E73" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -2591,7 +2732,7 @@
         <v>299</v>
       </c>
       <c r="E74" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -2608,7 +2749,7 @@
         <v>303</v>
       </c>
       <c r="E75" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2625,14 +2766,218 @@
         <v>307</v>
       </c>
       <c r="E76" t="s">
-        <v>10</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>308</v>
+      </c>
+      <c r="B77" t="s">
+        <v>309</v>
+      </c>
+      <c r="C77" t="s">
+        <v>310</v>
+      </c>
+      <c r="D77" t="s">
+        <v>311</v>
+      </c>
+      <c r="E77" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>313</v>
+      </c>
+      <c r="B78" t="s">
+        <v>314</v>
+      </c>
+      <c r="C78" t="s">
+        <v>315</v>
+      </c>
+      <c r="D78" t="s">
+        <v>316</v>
+      </c>
+      <c r="E78" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>317</v>
+      </c>
+      <c r="B79" t="s">
+        <v>318</v>
+      </c>
+      <c r="C79" t="s">
+        <v>319</v>
+      </c>
+      <c r="D79" t="s">
+        <v>320</v>
+      </c>
+      <c r="E79" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>321</v>
+      </c>
+      <c r="B80" t="s">
+        <v>322</v>
+      </c>
+      <c r="C80" t="s">
+        <v>323</v>
+      </c>
+      <c r="D80" t="s">
+        <v>324</v>
+      </c>
+      <c r="E80" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>325</v>
+      </c>
+      <c r="B81" t="s">
+        <v>326</v>
+      </c>
+      <c r="C81" t="s">
+        <v>327</v>
+      </c>
+      <c r="D81" t="s">
+        <v>328</v>
+      </c>
+      <c r="E81" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>329</v>
+      </c>
+      <c r="B82" t="s">
+        <v>330</v>
+      </c>
+      <c r="C82" t="s">
+        <v>331</v>
+      </c>
+      <c r="D82" t="s">
+        <v>332</v>
+      </c>
+      <c r="E82" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>333</v>
+      </c>
+      <c r="B83" t="s">
+        <v>334</v>
+      </c>
+      <c r="C83" t="s">
+        <v>335</v>
+      </c>
+      <c r="D83" t="s">
+        <v>336</v>
+      </c>
+      <c r="E83" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>337</v>
+      </c>
+      <c r="B84" t="s">
+        <v>338</v>
+      </c>
+      <c r="C84" t="s">
+        <v>339</v>
+      </c>
+      <c r="D84" t="s">
+        <v>340</v>
+      </c>
+      <c r="E84" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>341</v>
+      </c>
+      <c r="B85" t="s">
+        <v>342</v>
+      </c>
+      <c r="C85" t="s">
+        <v>343</v>
+      </c>
+      <c r="D85" t="s">
+        <v>344</v>
+      </c>
+      <c r="E85" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>345</v>
+      </c>
+      <c r="B86" t="s">
+        <v>346</v>
+      </c>
+      <c r="C86" t="s">
+        <v>347</v>
+      </c>
+      <c r="D86" t="s">
+        <v>348</v>
+      </c>
+      <c r="E86" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>349</v>
+      </c>
+      <c r="B87" t="s">
+        <v>350</v>
+      </c>
+      <c r="C87" t="s">
+        <v>351</v>
+      </c>
+      <c r="D87" t="s">
+        <v>352</v>
+      </c>
+      <c r="E87" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>353</v>
+      </c>
+      <c r="B88" t="s">
+        <v>354</v>
+      </c>
+      <c r="C88" t="s">
+        <v>355</v>
+      </c>
+      <c r="D88" t="s">
+        <v>356</v>
+      </c>
+      <c r="E88" t="s">
+        <v>312</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1768962967" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1769222744" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2641,16 +2986,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1768962967" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1768962967" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1768962967" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1768962967" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1769222744" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1769222744" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1769222744" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1769222744" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1768962967" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1769222744" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Add 10 new AppSumo apps: detailed reviews, category pages, and guide updates
- Added 10 new apps from AppSumo tracker (FormRobin, SuperCopy.ai, FlyMSG, WordHero, VanChat, Meet Oscar, VisualSitemaps, BrowserAct, Ethos, Awaz)
- Created detailed review pages (300+ lines each) with SEO optimization
- Updated reviews.html with all new apps
- Added apps to relevant category pages (writing-content, marketing-social, productivity-business, coding-development, voice-audio)
- Updated guide pages (best-lifetime-ai-tools, best-lifetime-deal-software-2026, lifetime-seo-tools, use-case guides)
- All reviews include pricing comparisons, features, pros/cons, FAQs, and affiliate links
</commit_message>
<xml_diff>
--- a/appsumo-affiliate-links-tracker.xlsx
+++ b/appsumo-affiliate-links-tracker.xlsx
@@ -13,19 +13,19 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1769222744" val="1068" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1769222744" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1769222744" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1769222744"/>
+      <pm:revision xmlns:pm="smNativeData" day="1769229861" val="1068" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1769229861" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1769229861" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1769229861"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="357">
-  <si>
-    <t>Product Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="396">
+  <si>
+    <t>https://appsumo.com/products/browseract/</t>
   </si>
   <si>
     <t>Product Slug</t>
@@ -961,139 +961,256 @@
     <t>https://appsumo.8odi.net/MAa2rP</t>
   </si>
   <si>
+    <t>MyClone</t>
+  </si>
+  <si>
+    <t>myclone</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/myclone/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/mOxjQD</t>
+  </si>
+  <si>
+    <t>Unmixr AI</t>
+  </si>
+  <si>
+    <t>unmixr-ai</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/unmixr-ai/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/PO1RP6</t>
+  </si>
+  <si>
+    <t>DREAMLIT</t>
+  </si>
+  <si>
+    <t>dreamlit-ai</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/dreamlit-ai/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/PO1RPq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Airbrush </t>
+  </si>
+  <si>
+    <t>airbrush-ai-image-generator</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/airbrush-ai-image-generator/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/XmzGVM</t>
+  </si>
+  <si>
+    <t>WPAutoBlog</t>
+  </si>
+  <si>
+    <t>wpautoblogcom</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/wpautoblogcom/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/090yeL</t>
+  </si>
+  <si>
+    <t>Tiny Talk</t>
+  </si>
+  <si>
+    <t>tiny-talk</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/tiny-talk/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/2anyAG</t>
+  </si>
+  <si>
+    <t>PISMO</t>
+  </si>
+  <si>
+    <t>pismo-alt</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/pismo-alt/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/dO4kQy</t>
+  </si>
+  <si>
+    <t>WebAbility.io</t>
+  </si>
+  <si>
+    <t>webabilityio</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/webabilityio/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/yqGj0y</t>
+  </si>
+  <si>
+    <t>Fynlo</t>
+  </si>
+  <si>
+    <t>fynlo</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/fynlo/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/YRWb6q</t>
+  </si>
+  <si>
+    <t>personeo.ai</t>
+  </si>
+  <si>
+    <t>personeoai</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/personeoai/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/K0kO1z</t>
+  </si>
+  <si>
+    <t>XInterview AI</t>
+  </si>
+  <si>
+    <t>xinterview</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/xinterview/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/7a3n2O</t>
+  </si>
+  <si>
+    <t>FormRobin</t>
+  </si>
+  <si>
+    <t>formrobin</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/formrobin/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/Z60LPz</t>
+  </si>
+  <si>
     <t>New</t>
   </si>
   <si>
-    <t>MyClone</t>
-  </si>
-  <si>
-    <t>myclone</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/myclone/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/mOxjQD</t>
-  </si>
-  <si>
-    <t>Unmixr AI</t>
-  </si>
-  <si>
-    <t>unmixr-ai</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/unmixr-ai/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/PO1RP6</t>
-  </si>
-  <si>
-    <t>DREAMLIT</t>
-  </si>
-  <si>
-    <t>dreamlit-ai</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/dreamlit-ai/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/PO1RPq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Airbrush </t>
-  </si>
-  <si>
-    <t>airbrush-ai-image-generator</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/airbrush-ai-image-generator/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/XmzGVM</t>
-  </si>
-  <si>
-    <t>WPAutoBlog</t>
-  </si>
-  <si>
-    <t>wpautoblogcom</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/wpautoblogcom/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/090yeL</t>
-  </si>
-  <si>
-    <t>Tiny Talk</t>
-  </si>
-  <si>
-    <t>tiny-talk</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/tiny-talk/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/2anyAG</t>
-  </si>
-  <si>
-    <t>PISMO</t>
-  </si>
-  <si>
-    <t>pismo-alt</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/pismo-alt/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/dO4kQy</t>
-  </si>
-  <si>
-    <t>WebAbility.io</t>
-  </si>
-  <si>
-    <t>webabilityio</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/webabilityio/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/yqGj0y</t>
-  </si>
-  <si>
-    <t>Fynlo</t>
-  </si>
-  <si>
-    <t>fynlo</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/fynlo/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/YRWb6q</t>
-  </si>
-  <si>
-    <t>personeo.ai</t>
-  </si>
-  <si>
-    <t>personeoai</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/personeoai/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/K0kO1z</t>
-  </si>
-  <si>
-    <t>XInterview AI</t>
-  </si>
-  <si>
-    <t>xinterview</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/xinterview/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/7a3n2O</t>
+    <t>SuperCopy.ai</t>
+  </si>
+  <si>
+    <t>supercopy-ai</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/supercopy-ai/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/o4Q5jW</t>
+  </si>
+  <si>
+    <t>FlyMSG</t>
+  </si>
+  <si>
+    <t>flymsg</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/flymsg/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/090ykN</t>
+  </si>
+  <si>
+    <t>WordHero</t>
+  </si>
+  <si>
+    <t>marketplace-wordhero</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/marketplace-wordhero/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/bORPWM</t>
+  </si>
+  <si>
+    <t>VanChat</t>
+  </si>
+  <si>
+    <t>vanchat</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/vanchat/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/vPeQoL</t>
+  </si>
+  <si>
+    <t>Meet Oscar</t>
+  </si>
+  <si>
+    <t>meet-oscar</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/meet-oscar/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/YRWbrr</t>
+  </si>
+  <si>
+    <t>VisualSitemaps</t>
+  </si>
+  <si>
+    <t>visualsitemaps</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/visualsitemaps/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/qzrODg</t>
+  </si>
+  <si>
+    <t>BrowserAct</t>
+  </si>
+  <si>
+    <t>browseract</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/xLAzEy</t>
+  </si>
+  <si>
+    <t>Ethos</t>
+  </si>
+  <si>
+    <t>ethos</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/ethos/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/DyDR0b</t>
+  </si>
+  <si>
+    <t>Awaz</t>
+  </si>
+  <si>
+    <t>awaz</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/awaz/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/QjV2P6</t>
   </si>
 </sst>
 </file>
@@ -1118,7 +1235,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1769222744" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1769229861" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -1140,7 +1257,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1769222744" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1769229861" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1162,7 +1279,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1769222744"/>
+          <pm:border xmlns:pm="smNativeData" id="1769229861"/>
         </ext>
       </extLst>
     </border>
@@ -1181,7 +1298,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1769222744"/>
+          <pm:border xmlns:pm="smNativeData" id="1769229861"/>
         </ext>
       </extLst>
     </border>
@@ -1198,7 +1315,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1769222744" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1769229861" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -1462,10 +1579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:F88"/>
+  <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -1477,7 +1594,7 @@
     <col min="5" max="5" width="10.000000" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1528,7 +1645,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -2783,201 +2900,388 @@
         <v>311</v>
       </c>
       <c r="E77" t="s">
-        <v>312</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
+        <v>312</v>
+      </c>
+      <c r="B78" t="s">
         <v>313</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" t="s">
         <v>314</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
         <v>315</v>
       </c>
-      <c r="D78" t="s">
-        <v>316</v>
-      </c>
       <c r="E78" t="s">
-        <v>312</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" t="s">
+        <v>316</v>
+      </c>
+      <c r="B79" t="s">
         <v>317</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" t="s">
         <v>318</v>
       </c>
-      <c r="C79" t="s">
+      <c r="D79" t="s">
         <v>319</v>
       </c>
-      <c r="D79" t="s">
-        <v>320</v>
-      </c>
       <c r="E79" t="s">
-        <v>312</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
+        <v>320</v>
+      </c>
+      <c r="B80" t="s">
         <v>321</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" t="s">
         <v>322</v>
       </c>
-      <c r="C80" t="s">
+      <c r="D80" t="s">
         <v>323</v>
       </c>
-      <c r="D80" t="s">
-        <v>324</v>
-      </c>
       <c r="E80" t="s">
-        <v>312</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
+        <v>324</v>
+      </c>
+      <c r="B81" t="s">
         <v>325</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" t="s">
         <v>326</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" t="s">
         <v>327</v>
       </c>
-      <c r="D81" t="s">
-        <v>328</v>
-      </c>
       <c r="E81" t="s">
-        <v>312</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" t="s">
+        <v>328</v>
+      </c>
+      <c r="B82" t="s">
         <v>329</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" t="s">
         <v>330</v>
       </c>
-      <c r="C82" t="s">
+      <c r="D82" t="s">
         <v>331</v>
       </c>
-      <c r="D82" t="s">
-        <v>332</v>
-      </c>
       <c r="E82" t="s">
-        <v>312</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
+        <v>332</v>
+      </c>
+      <c r="B83" t="s">
         <v>333</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" t="s">
         <v>334</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
         <v>335</v>
       </c>
-      <c r="D83" t="s">
-        <v>336</v>
-      </c>
       <c r="E83" t="s">
-        <v>312</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
+        <v>336</v>
+      </c>
+      <c r="B84" t="s">
         <v>337</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" t="s">
         <v>338</v>
       </c>
-      <c r="C84" t="s">
+      <c r="D84" t="s">
         <v>339</v>
       </c>
-      <c r="D84" t="s">
-        <v>340</v>
-      </c>
       <c r="E84" t="s">
-        <v>312</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
+        <v>340</v>
+      </c>
+      <c r="B85" t="s">
         <v>341</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" t="s">
         <v>342</v>
       </c>
-      <c r="C85" t="s">
+      <c r="D85" t="s">
         <v>343</v>
       </c>
-      <c r="D85" t="s">
-        <v>344</v>
-      </c>
       <c r="E85" t="s">
-        <v>312</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
+        <v>344</v>
+      </c>
+      <c r="B86" t="s">
         <v>345</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" t="s">
         <v>346</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
         <v>347</v>
       </c>
-      <c r="D86" t="s">
-        <v>348</v>
-      </c>
       <c r="E86" t="s">
-        <v>312</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
+        <v>348</v>
+      </c>
+      <c r="B87" t="s">
         <v>349</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" t="s">
         <v>350</v>
       </c>
-      <c r="C87" t="s">
+      <c r="D87" t="s">
         <v>351</v>
       </c>
-      <c r="D87" t="s">
-        <v>352</v>
-      </c>
       <c r="E87" t="s">
-        <v>312</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
+        <v>352</v>
+      </c>
+      <c r="B88" t="s">
         <v>353</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" t="s">
         <v>354</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
         <v>355</v>
       </c>
-      <c r="D88" t="s">
+      <c r="E88" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
         <v>356</v>
       </c>
-      <c r="E88" t="s">
-        <v>312</v>
+      <c r="B89" t="s">
+        <v>357</v>
+      </c>
+      <c r="C89" t="s">
+        <v>358</v>
+      </c>
+      <c r="D89" t="s">
+        <v>359</v>
+      </c>
+      <c r="E89" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>361</v>
+      </c>
+      <c r="B90" t="s">
+        <v>362</v>
+      </c>
+      <c r="C90" t="s">
+        <v>363</v>
+      </c>
+      <c r="D90" t="s">
+        <v>364</v>
+      </c>
+      <c r="E90" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>365</v>
+      </c>
+      <c r="B91" t="s">
+        <v>366</v>
+      </c>
+      <c r="C91" t="s">
+        <v>367</v>
+      </c>
+      <c r="D91" t="s">
+        <v>368</v>
+      </c>
+      <c r="E91" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" t="s">
+        <v>369</v>
+      </c>
+      <c r="B92" t="s">
+        <v>370</v>
+      </c>
+      <c r="C92" t="s">
+        <v>371</v>
+      </c>
+      <c r="D92" t="s">
+        <v>372</v>
+      </c>
+      <c r="E92" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" t="s">
+        <v>373</v>
+      </c>
+      <c r="B93" t="s">
+        <v>374</v>
+      </c>
+      <c r="C93" t="s">
+        <v>375</v>
+      </c>
+      <c r="D93" t="s">
+        <v>376</v>
+      </c>
+      <c r="E93" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" t="s">
+        <v>377</v>
+      </c>
+      <c r="B94" t="s">
+        <v>378</v>
+      </c>
+      <c r="C94" t="s">
+        <v>379</v>
+      </c>
+      <c r="D94" t="s">
+        <v>380</v>
+      </c>
+      <c r="E94" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" t="s">
+        <v>10</v>
+      </c>
+      <c r="B95" t="s">
+        <v>11</v>
+      </c>
+      <c r="C95" t="s">
+        <v>12</v>
+      </c>
+      <c r="D95" t="s">
+        <v>13</v>
+      </c>
+      <c r="E95" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" t="s">
+        <v>381</v>
+      </c>
+      <c r="B96" t="s">
+        <v>382</v>
+      </c>
+      <c r="C96" t="s">
+        <v>383</v>
+      </c>
+      <c r="D96" t="s">
+        <v>384</v>
+      </c>
+      <c r="E96" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" t="s">
+        <v>385</v>
+      </c>
+      <c r="B97" t="s">
+        <v>386</v>
+      </c>
+      <c r="C97" t="s">
+        <v>0</v>
+      </c>
+      <c r="D97" t="s">
+        <v>387</v>
+      </c>
+      <c r="E97" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>388</v>
+      </c>
+      <c r="B98" t="s">
+        <v>389</v>
+      </c>
+      <c r="C98" t="s">
+        <v>390</v>
+      </c>
+      <c r="D98" t="s">
+        <v>391</v>
+      </c>
+      <c r="E98" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>392</v>
+      </c>
+      <c r="B99" t="s">
+        <v>393</v>
+      </c>
+      <c r="C99" t="s">
+        <v>394</v>
+      </c>
+      <c r="D99" t="s">
+        <v>395</v>
+      </c>
+      <c r="E99" t="s">
+        <v>360</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1769222744" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1769229861" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2986,16 +3290,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1769222744" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1769222744" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1769222744" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1769222744" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1769229861" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1769229861" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1769229861" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1769229861" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1769222744" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1769229861" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Add 29 new AppSumo apps: detailed reviews, category pages, and guide updates
- Created 29 comprehensive review pages (300+ lines each) with SEO optimization
- Added all apps to reviews.html tools array with proper categorization
- Integrated apps into relevant category pages (writing, marketing, productivity, design, coding, voice, research, analytics)
- Added apps to guide pages (best-lifetime-deal-software-2026, best-lifetime-ai-tools, lifetime-seo-tools)
- All affiliate links verified and correctly linked
- Apps include: SheetX AI, ClickMoat, WriteSeed AI, Quizify, Kvitly, Fox Signals, BizReply, Laxis AI, Wordplay, Headshotly AI, Power Formulas, No-Code MBA, Learniverse, Yazo AI, Seopital, ImageColorizer, Viinyx, SpeechActors, SheetGPT, WhatsApp Widget, Equitest, OnlineCourseHost, Creative Score, Airfive, Bugsmash, Reoon, Screpy, Vocal, IdeaBuddy
</commit_message>
<xml_diff>
--- a/appsumo-affiliate-links-tracker.xlsx
+++ b/appsumo-affiliate-links-tracker.xlsx
@@ -13,17 +13,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1769229861" val="1068" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1769229861" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1769229861" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1769229861"/>
+      <pm:revision xmlns:pm="smNativeData" day="1769234578" val="1068" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1769234578" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1769234578" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1769234578"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="507">
   <si>
     <t>https://appsumo.com/products/browseract/</t>
   </si>
@@ -1105,112 +1105,445 @@
     <t>https://appsumo.8odi.net/Z60LPz</t>
   </si>
   <si>
+    <t>SuperCopy.ai</t>
+  </si>
+  <si>
+    <t>supercopy-ai</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/supercopy-ai/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/o4Q5jW</t>
+  </si>
+  <si>
+    <t>FlyMSG</t>
+  </si>
+  <si>
+    <t>flymsg</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/flymsg/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/090ykN</t>
+  </si>
+  <si>
+    <t>WordHero</t>
+  </si>
+  <si>
+    <t>marketplace-wordhero</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/marketplace-wordhero/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/bORPWM</t>
+  </si>
+  <si>
+    <t>VanChat</t>
+  </si>
+  <si>
+    <t>vanchat</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/vanchat/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/vPeQoL</t>
+  </si>
+  <si>
+    <t>Meet Oscar</t>
+  </si>
+  <si>
+    <t>meet-oscar</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/meet-oscar/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/YRWbrr</t>
+  </si>
+  <si>
+    <t>VisualSitemaps</t>
+  </si>
+  <si>
+    <t>visualsitemaps</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/visualsitemaps/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/qzrODg</t>
+  </si>
+  <si>
+    <t>BrowserAct</t>
+  </si>
+  <si>
+    <t>browseract</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/xLAzEy</t>
+  </si>
+  <si>
+    <t>Ethos</t>
+  </si>
+  <si>
+    <t>ethos</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/ethos/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/DyDR0b</t>
+  </si>
+  <si>
+    <t>Awaz</t>
+  </si>
+  <si>
+    <t>awaz</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/awaz/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/QjV2P6</t>
+  </si>
+  <si>
+    <t>SheetXAI</t>
+  </si>
+  <si>
+    <t>sheetxai</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/sheetxai/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/e1dkKD</t>
+  </si>
+  <si>
     <t>New</t>
   </si>
   <si>
-    <t>SuperCopy.ai</t>
-  </si>
-  <si>
-    <t>supercopy-ai</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/supercopy-ai/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/o4Q5jW</t>
-  </si>
-  <si>
-    <t>FlyMSG</t>
-  </si>
-  <si>
-    <t>flymsg</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/flymsg/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/090ykN</t>
-  </si>
-  <si>
-    <t>WordHero</t>
-  </si>
-  <si>
-    <t>marketplace-wordhero</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/marketplace-wordhero/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/bORPWM</t>
-  </si>
-  <si>
-    <t>VanChat</t>
-  </si>
-  <si>
-    <t>vanchat</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/vanchat/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/vPeQoL</t>
-  </si>
-  <si>
-    <t>Meet Oscar</t>
-  </si>
-  <si>
-    <t>meet-oscar</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/meet-oscar/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/YRWbrr</t>
-  </si>
-  <si>
-    <t>VisualSitemaps</t>
-  </si>
-  <si>
-    <t>visualsitemaps</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/visualsitemaps/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/qzrODg</t>
-  </si>
-  <si>
-    <t>BrowserAct</t>
-  </si>
-  <si>
-    <t>browseract</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/xLAzEy</t>
-  </si>
-  <si>
-    <t>Ethos</t>
-  </si>
-  <si>
-    <t>ethos</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/ethos/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/DyDR0b</t>
-  </si>
-  <si>
-    <t>Awaz</t>
-  </si>
-  <si>
-    <t>awaz</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/awaz/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/QjV2P6</t>
+    <t>Clickmoat</t>
+  </si>
+  <si>
+    <t>clickmoat</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/clickmoat/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/APLRWx</t>
+  </si>
+  <si>
+    <t>Writeseed</t>
+  </si>
+  <si>
+    <t>writeseed-ai-content-writer</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/writeseed-ai-content-writer/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/19EZra</t>
+  </si>
+  <si>
+    <t>Quizify</t>
+  </si>
+  <si>
+    <t>quizify</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/quizify/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/Vxo2xa</t>
+  </si>
+  <si>
+    <t>Kvitly</t>
+  </si>
+  <si>
+    <t>kvitly</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/kvitly/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/Z60Y6Q</t>
+  </si>
+  <si>
+    <t>Fox Signals</t>
+  </si>
+  <si>
+    <t>fox-signals</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/fox-signals/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/gOyaOO</t>
+  </si>
+  <si>
+    <t>Bizreply</t>
+  </si>
+  <si>
+    <t>Laxis.ai</t>
+  </si>
+  <si>
+    <t>laxis-ai</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/laxis-ai-prospect-research/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/Xmz2m4</t>
+  </si>
+  <si>
+    <t>Wordplay</t>
+  </si>
+  <si>
+    <t>wordplay</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/wordplay-long-form-ai-writer/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/BnqRnx</t>
+  </si>
+  <si>
+    <t>Headshotly.ai</t>
+  </si>
+  <si>
+    <t>headshotly-ai</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/headshotly-ai/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/bORjOP</t>
+  </si>
+  <si>
+    <t>Power Formulas</t>
+  </si>
+  <si>
+    <t>power-formulas</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/power-formulas/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/3JbmJX</t>
+  </si>
+  <si>
+    <t>No Code Mba</t>
+  </si>
+  <si>
+    <t>no-code-mba-deal</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/no-code-mba-deal/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/dO45Oq</t>
+  </si>
+  <si>
+    <t>Learniverse</t>
+  </si>
+  <si>
+    <t>learniverse</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/learniverse/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/yqG4qv</t>
+  </si>
+  <si>
+    <t>Yazo.ai</t>
+  </si>
+  <si>
+    <t>yazo-ai</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/yazo-ai-content-generator/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/K0ky0A</t>
+  </si>
+  <si>
+    <t>Seopital</t>
+  </si>
+  <si>
+    <t>seopital</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/seopital/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/LKeRKL</t>
+  </si>
+  <si>
+    <t>Image Colorizer</t>
+  </si>
+  <si>
+    <t>imagecolorizer</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/imagecolorizer/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/qzrOzj</t>
+  </si>
+  <si>
+    <t>Viinyx</t>
+  </si>
+  <si>
+    <t>viinyx</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/viinyx/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/xLAzLd</t>
+  </si>
+  <si>
+    <t>Speechactors</t>
+  </si>
+  <si>
+    <t>speechactors</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/speechactors/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/rajJa5</t>
+  </si>
+  <si>
+    <t>Sheetgpt</t>
+  </si>
+  <si>
+    <t>sheetgpt</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/sheetgpt-chatgpt-google-sheets-integration/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/jeKJev</t>
+  </si>
+  <si>
+    <t>Whatsapp Widget</t>
+  </si>
+  <si>
+    <t>marketplace-whatsapp-widget</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/marketplace-whatsapp-widget/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/PO1mOX</t>
+  </si>
+  <si>
+    <t>Equitest</t>
+  </si>
+  <si>
+    <t>equitest</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/marketplace-equitest-online-valuation-platform/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/kOLJOn</t>
+  </si>
+  <si>
+    <t>OnlineCourseHost</t>
+  </si>
+  <si>
+    <t>onlinecoursehost</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/onlinecoursehost/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/GKrRKr</t>
+  </si>
+  <si>
+    <t>CreativeScore</t>
+  </si>
+  <si>
+    <t>creative-score</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/creative-score/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/19EZ9a</t>
+  </si>
+  <si>
+    <t>Airfive</t>
+  </si>
+  <si>
+    <t>airfive</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/airfive/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/Vxo2Oa</t>
+  </si>
+  <si>
+    <t>Bugsmash</t>
+  </si>
+  <si>
+    <t>bugsmash</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/bugsmash/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/JK5Rkr</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/reoon-email-verifier/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/Z60YVQ</t>
+  </si>
+  <si>
+    <t>Screpy</t>
+  </si>
+  <si>
+    <t>screpy</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/screpy/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/BnqR5x</t>
+  </si>
+  <si>
+    <t>Vocal</t>
+  </si>
+  <si>
+    <t>marketplace-vocal</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/marketplace-vocal/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/zx1nze</t>
+  </si>
+  <si>
+    <t>IdeaBuddy</t>
+  </si>
+  <si>
+    <t>marketplace-ideabuddy</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/marketplace-ideabuddy/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/EEQR0e</t>
   </si>
 </sst>
 </file>
@@ -1235,7 +1568,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1769229861" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1769234578" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -1257,7 +1590,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1769229861" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1769234578" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1279,7 +1612,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1769229861"/>
+          <pm:border xmlns:pm="smNativeData" id="1769234578"/>
         </ext>
       </extLst>
     </border>
@@ -1298,7 +1631,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1769229861"/>
+          <pm:border xmlns:pm="smNativeData" id="1769234578"/>
         </ext>
       </extLst>
     </border>
@@ -1315,7 +1648,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1769229861" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1769234578" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -1579,10 +1912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E128"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -3104,92 +3437,92 @@
         <v>359</v>
       </c>
       <c r="E89" t="s">
-        <v>360</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
+        <v>360</v>
+      </c>
+      <c r="B90" t="s">
         <v>361</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
         <v>362</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D90" t="s">
         <v>363</v>
       </c>
-      <c r="D90" t="s">
-        <v>364</v>
-      </c>
       <c r="E90" t="s">
-        <v>360</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
+        <v>364</v>
+      </c>
+      <c r="B91" t="s">
         <v>365</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" t="s">
         <v>366</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
         <v>367</v>
       </c>
-      <c r="D91" t="s">
-        <v>368</v>
-      </c>
       <c r="E91" t="s">
-        <v>360</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
+        <v>368</v>
+      </c>
+      <c r="B92" t="s">
         <v>369</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
         <v>370</v>
       </c>
-      <c r="C92" t="s">
+      <c r="D92" t="s">
         <v>371</v>
       </c>
-      <c r="D92" t="s">
-        <v>372</v>
-      </c>
       <c r="E92" t="s">
-        <v>360</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
+        <v>372</v>
+      </c>
+      <c r="B93" t="s">
         <v>373</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93" t="s">
         <v>374</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D93" t="s">
         <v>375</v>
       </c>
-      <c r="D93" t="s">
-        <v>376</v>
-      </c>
       <c r="E93" t="s">
-        <v>360</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
+        <v>376</v>
+      </c>
+      <c r="B94" t="s">
         <v>377</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" t="s">
         <v>378</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D94" t="s">
         <v>379</v>
       </c>
-      <c r="D94" t="s">
-        <v>380</v>
-      </c>
       <c r="E94" t="s">
-        <v>360</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -3206,82 +3539,575 @@
         <v>13</v>
       </c>
       <c r="E95" t="s">
-        <v>360</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" t="s">
+        <v>380</v>
+      </c>
+      <c r="B96" t="s">
         <v>381</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C96" t="s">
         <v>382</v>
       </c>
-      <c r="C96" t="s">
+      <c r="D96" t="s">
         <v>383</v>
       </c>
-      <c r="D96" t="s">
-        <v>384</v>
-      </c>
       <c r="E96" t="s">
-        <v>360</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" t="s">
+        <v>384</v>
+      </c>
+      <c r="B97" t="s">
         <v>385</v>
-      </c>
-      <c r="B97" t="s">
-        <v>386</v>
       </c>
       <c r="C97" t="s">
         <v>0</v>
       </c>
       <c r="D97" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E97" t="s">
-        <v>360</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" t="s">
+        <v>387</v>
+      </c>
+      <c r="B98" t="s">
         <v>388</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" t="s">
         <v>389</v>
       </c>
-      <c r="C98" t="s">
+      <c r="D98" t="s">
         <v>390</v>
       </c>
-      <c r="D98" t="s">
-        <v>391</v>
-      </c>
       <c r="E98" t="s">
-        <v>360</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" t="s">
+        <v>391</v>
+      </c>
+      <c r="B99" t="s">
         <v>392</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" t="s">
         <v>393</v>
       </c>
-      <c r="C99" t="s">
+      <c r="D99" t="s">
         <v>394</v>
       </c>
-      <c r="D99" t="s">
+      <c r="E99" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
         <v>395</v>
       </c>
-      <c r="E99" t="s">
-        <v>360</v>
+      <c r="B100" t="s">
+        <v>396</v>
+      </c>
+      <c r="C100" t="s">
+        <v>397</v>
+      </c>
+      <c r="D100" t="s">
+        <v>398</v>
+      </c>
+      <c r="E100" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>400</v>
+      </c>
+      <c r="B101" t="s">
+        <v>401</v>
+      </c>
+      <c r="C101" t="s">
+        <v>402</v>
+      </c>
+      <c r="D101" t="s">
+        <v>403</v>
+      </c>
+      <c r="E101" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" t="s">
+        <v>404</v>
+      </c>
+      <c r="B102" t="s">
+        <v>405</v>
+      </c>
+      <c r="C102" t="s">
+        <v>406</v>
+      </c>
+      <c r="D102" t="s">
+        <v>407</v>
+      </c>
+      <c r="E102" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" t="s">
+        <v>408</v>
+      </c>
+      <c r="B103" t="s">
+        <v>409</v>
+      </c>
+      <c r="C103" t="s">
+        <v>410</v>
+      </c>
+      <c r="D103" t="s">
+        <v>411</v>
+      </c>
+      <c r="E103" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" t="s">
+        <v>412</v>
+      </c>
+      <c r="B104" t="s">
+        <v>413</v>
+      </c>
+      <c r="C104" t="s">
+        <v>414</v>
+      </c>
+      <c r="D104" t="s">
+        <v>415</v>
+      </c>
+      <c r="E104" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" t="s">
+        <v>416</v>
+      </c>
+      <c r="B105" t="s">
+        <v>417</v>
+      </c>
+      <c r="C105" t="s">
+        <v>418</v>
+      </c>
+      <c r="D105" t="s">
+        <v>419</v>
+      </c>
+      <c r="E105" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" t="s">
+        <v>420</v>
+      </c>
+      <c r="B106" t="s">
+        <v>57</v>
+      </c>
+      <c r="C106" t="s">
+        <v>58</v>
+      </c>
+      <c r="D106" t="s">
+        <v>59</v>
+      </c>
+      <c r="E106" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" t="s">
+        <v>421</v>
+      </c>
+      <c r="B107" t="s">
+        <v>422</v>
+      </c>
+      <c r="C107" t="s">
+        <v>423</v>
+      </c>
+      <c r="D107" t="s">
+        <v>424</v>
+      </c>
+      <c r="E107" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" t="s">
+        <v>425</v>
+      </c>
+      <c r="B108" t="s">
+        <v>426</v>
+      </c>
+      <c r="C108" t="s">
+        <v>427</v>
+      </c>
+      <c r="D108" t="s">
+        <v>428</v>
+      </c>
+      <c r="E108" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" t="s">
+        <v>429</v>
+      </c>
+      <c r="B109" t="s">
+        <v>430</v>
+      </c>
+      <c r="C109" t="s">
+        <v>431</v>
+      </c>
+      <c r="D109" t="s">
+        <v>432</v>
+      </c>
+      <c r="E109" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" t="s">
+        <v>433</v>
+      </c>
+      <c r="B110" t="s">
+        <v>434</v>
+      </c>
+      <c r="C110" t="s">
+        <v>435</v>
+      </c>
+      <c r="D110" t="s">
+        <v>436</v>
+      </c>
+      <c r="E110" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" t="s">
+        <v>437</v>
+      </c>
+      <c r="B111" t="s">
+        <v>438</v>
+      </c>
+      <c r="C111" t="s">
+        <v>439</v>
+      </c>
+      <c r="D111" t="s">
+        <v>440</v>
+      </c>
+      <c r="E111" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
+      <c r="A112" t="s">
+        <v>441</v>
+      </c>
+      <c r="B112" t="s">
+        <v>442</v>
+      </c>
+      <c r="C112" t="s">
+        <v>443</v>
+      </c>
+      <c r="D112" t="s">
+        <v>444</v>
+      </c>
+      <c r="E112" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" t="s">
+        <v>445</v>
+      </c>
+      <c r="B113" t="s">
+        <v>446</v>
+      </c>
+      <c r="C113" t="s">
+        <v>447</v>
+      </c>
+      <c r="D113" t="s">
+        <v>448</v>
+      </c>
+      <c r="E113" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" t="s">
+        <v>449</v>
+      </c>
+      <c r="B114" t="s">
+        <v>450</v>
+      </c>
+      <c r="C114" t="s">
+        <v>451</v>
+      </c>
+      <c r="D114" t="s">
+        <v>452</v>
+      </c>
+      <c r="E114" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" t="s">
+        <v>453</v>
+      </c>
+      <c r="B115" t="s">
+        <v>454</v>
+      </c>
+      <c r="C115" t="s">
+        <v>455</v>
+      </c>
+      <c r="D115" t="s">
+        <v>456</v>
+      </c>
+      <c r="E115" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" t="s">
+        <v>457</v>
+      </c>
+      <c r="B116" t="s">
+        <v>458</v>
+      </c>
+      <c r="C116" t="s">
+        <v>459</v>
+      </c>
+      <c r="D116" t="s">
+        <v>460</v>
+      </c>
+      <c r="E116" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" t="s">
+        <v>461</v>
+      </c>
+      <c r="B117" t="s">
+        <v>462</v>
+      </c>
+      <c r="C117" t="s">
+        <v>463</v>
+      </c>
+      <c r="D117" t="s">
+        <v>464</v>
+      </c>
+      <c r="E117" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" t="s">
+        <v>465</v>
+      </c>
+      <c r="B118" t="s">
+        <v>466</v>
+      </c>
+      <c r="C118" t="s">
+        <v>467</v>
+      </c>
+      <c r="D118" t="s">
+        <v>468</v>
+      </c>
+      <c r="E118" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" t="s">
+        <v>469</v>
+      </c>
+      <c r="B119" t="s">
+        <v>470</v>
+      </c>
+      <c r="C119" t="s">
+        <v>471</v>
+      </c>
+      <c r="D119" t="s">
+        <v>472</v>
+      </c>
+      <c r="E119" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" t="s">
+        <v>473</v>
+      </c>
+      <c r="B120" t="s">
+        <v>474</v>
+      </c>
+      <c r="C120" t="s">
+        <v>475</v>
+      </c>
+      <c r="D120" t="s">
+        <v>476</v>
+      </c>
+      <c r="E120" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
+      <c r="A121" t="s">
+        <v>477</v>
+      </c>
+      <c r="B121" t="s">
+        <v>478</v>
+      </c>
+      <c r="C121" t="s">
+        <v>479</v>
+      </c>
+      <c r="D121" t="s">
+        <v>480</v>
+      </c>
+      <c r="E121" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" t="s">
+        <v>481</v>
+      </c>
+      <c r="B122" t="s">
+        <v>482</v>
+      </c>
+      <c r="C122" t="s">
+        <v>483</v>
+      </c>
+      <c r="D122" t="s">
+        <v>484</v>
+      </c>
+      <c r="E122" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" t="s">
+        <v>485</v>
+      </c>
+      <c r="B123" t="s">
+        <v>486</v>
+      </c>
+      <c r="C123" t="s">
+        <v>487</v>
+      </c>
+      <c r="D123" t="s">
+        <v>488</v>
+      </c>
+      <c r="E123" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" t="s">
+        <v>489</v>
+      </c>
+      <c r="B124" t="s">
+        <v>490</v>
+      </c>
+      <c r="C124" t="s">
+        <v>491</v>
+      </c>
+      <c r="D124" t="s">
+        <v>492</v>
+      </c>
+      <c r="E124" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" t="s">
+        <v>228</v>
+      </c>
+      <c r="B125" t="s">
+        <v>229</v>
+      </c>
+      <c r="C125" t="s">
+        <v>493</v>
+      </c>
+      <c r="D125" t="s">
+        <v>494</v>
+      </c>
+      <c r="E125" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" t="s">
+        <v>495</v>
+      </c>
+      <c r="B126" t="s">
+        <v>496</v>
+      </c>
+      <c r="C126" t="s">
+        <v>497</v>
+      </c>
+      <c r="D126" t="s">
+        <v>498</v>
+      </c>
+      <c r="E126" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" t="s">
+        <v>499</v>
+      </c>
+      <c r="B127" t="s">
+        <v>500</v>
+      </c>
+      <c r="C127" t="s">
+        <v>501</v>
+      </c>
+      <c r="D127" t="s">
+        <v>502</v>
+      </c>
+      <c r="E127" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" t="s">
+        <v>503</v>
+      </c>
+      <c r="B128" t="s">
+        <v>504</v>
+      </c>
+      <c r="C128" t="s">
+        <v>505</v>
+      </c>
+      <c r="D128" t="s">
+        <v>506</v>
+      </c>
+      <c r="E128" t="s">
+        <v>399</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1769229861" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1769234578" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -3290,16 +4116,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1769229861" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1769229861" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1769229861" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1769229861" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1769234578" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1769234578" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1769234578" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1769234578" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1769229861" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1769234578" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Add 57 New AppSumo apps: reviews, guides, best-of, blogs, sitemap
- Add 57 New apps from tracker to reviews.html, create detailed tool review pages
- New guide: best-new-appsumo-deals-2026.html; update best-lifetime-ai-tools, best-appsumo-ai-deals
- Add New AppSumo sections to best-ai-voice-generators, best-ai-blog-writing-tools, best-ai-photo-editing-tools, best-ai-tools-for-data-analysis
- New blogs: 57 New AppSumo Deals 2026, Best New AppSumo Deals for Writers and Designers 2026; add to blog.html
- Update sitemap with new tool URLs, guide, and blogs
- Scripts: add_new_appsumo_apps.py, apply_new_apps_to_site.py, new_apps_data.json
</commit_message>
<xml_diff>
--- a/appsumo-affiliate-links-tracker.xlsx
+++ b/appsumo-affiliate-links-tracker.xlsx
@@ -13,17 +13,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1769234578" val="1068" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1769234578" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1769234578" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1769234578"/>
+      <pm:revision xmlns:pm="smNativeData" day="1769355031" val="1068" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1769355031" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1769355031" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1769355031"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="734">
   <si>
     <t>https://appsumo.com/products/browseract/</t>
   </si>
@@ -1222,328 +1222,1009 @@
     <t>https://appsumo.8odi.net/e1dkKD</t>
   </si>
   <si>
+    <t>Clickmoat</t>
+  </si>
+  <si>
+    <t>clickmoat</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/clickmoat/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/APLRWx</t>
+  </si>
+  <si>
+    <t>Writeseed</t>
+  </si>
+  <si>
+    <t>writeseed-ai-content-writer</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/writeseed-ai-content-writer/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/19EZra</t>
+  </si>
+  <si>
+    <t>Quizify</t>
+  </si>
+  <si>
+    <t>quizify</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/quizify/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/Vxo2xa</t>
+  </si>
+  <si>
+    <t>Kvitly</t>
+  </si>
+  <si>
+    <t>kvitly</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/kvitly/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/Z60Y6Q</t>
+  </si>
+  <si>
+    <t>Fox Signals</t>
+  </si>
+  <si>
+    <t>fox-signals</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/fox-signals/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/gOyaOO</t>
+  </si>
+  <si>
+    <t>Bizreply</t>
+  </si>
+  <si>
+    <t>Laxis.ai</t>
+  </si>
+  <si>
+    <t>laxis-ai</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/laxis-ai-prospect-research/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/Xmz2m4</t>
+  </si>
+  <si>
+    <t>Wordplay</t>
+  </si>
+  <si>
+    <t>wordplay</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/wordplay-long-form-ai-writer/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/BnqRnx</t>
+  </si>
+  <si>
+    <t>Headshotly.ai</t>
+  </si>
+  <si>
+    <t>headshotly-ai</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/headshotly-ai/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/bORjOP</t>
+  </si>
+  <si>
+    <t>Power Formulas</t>
+  </si>
+  <si>
+    <t>power-formulas</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/power-formulas/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/3JbmJX</t>
+  </si>
+  <si>
+    <t>No Code Mba</t>
+  </si>
+  <si>
+    <t>no-code-mba-deal</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/no-code-mba-deal/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/dO45Oq</t>
+  </si>
+  <si>
+    <t>Learniverse</t>
+  </si>
+  <si>
+    <t>learniverse</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/learniverse/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/yqG4qv</t>
+  </si>
+  <si>
+    <t>Yazo.ai</t>
+  </si>
+  <si>
+    <t>yazo-ai</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/yazo-ai-content-generator/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/K0ky0A</t>
+  </si>
+  <si>
+    <t>Seopital</t>
+  </si>
+  <si>
+    <t>seopital</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/seopital/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/LKeRKL</t>
+  </si>
+  <si>
+    <t>Image Colorizer</t>
+  </si>
+  <si>
+    <t>imagecolorizer</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/imagecolorizer/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/qzrOzj</t>
+  </si>
+  <si>
+    <t>Viinyx</t>
+  </si>
+  <si>
+    <t>viinyx</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/viinyx/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/xLAzLd</t>
+  </si>
+  <si>
+    <t>Speechactors</t>
+  </si>
+  <si>
+    <t>speechactors</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/speechactors/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/rajJa5</t>
+  </si>
+  <si>
+    <t>Sheetgpt</t>
+  </si>
+  <si>
+    <t>sheetgpt</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/sheetgpt-chatgpt-google-sheets-integration/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/jeKJev</t>
+  </si>
+  <si>
+    <t>Whatsapp Widget</t>
+  </si>
+  <si>
+    <t>marketplace-whatsapp-widget</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/marketplace-whatsapp-widget/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/PO1mOX</t>
+  </si>
+  <si>
+    <t>Equitest</t>
+  </si>
+  <si>
+    <t>equitest</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/marketplace-equitest-online-valuation-platform/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/kOLJOn</t>
+  </si>
+  <si>
+    <t>OnlineCourseHost</t>
+  </si>
+  <si>
+    <t>onlinecoursehost</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/onlinecoursehost/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/GKrRKr</t>
+  </si>
+  <si>
+    <t>CreativeScore</t>
+  </si>
+  <si>
+    <t>creative-score</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/creative-score/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/19EZ9a</t>
+  </si>
+  <si>
+    <t>Airfive</t>
+  </si>
+  <si>
+    <t>airfive</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/airfive/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/Vxo2Oa</t>
+  </si>
+  <si>
+    <t>Bugsmash</t>
+  </si>
+  <si>
+    <t>bugsmash</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/bugsmash/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/JK5Rkr</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/reoon-email-verifier/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/Z60YVQ</t>
+  </si>
+  <si>
+    <t>Screpy</t>
+  </si>
+  <si>
+    <t>screpy</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/screpy/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/BnqR5x</t>
+  </si>
+  <si>
+    <t>Vocal</t>
+  </si>
+  <si>
+    <t>marketplace-vocal</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/marketplace-vocal/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/zx1nze</t>
+  </si>
+  <si>
+    <t>IdeaBuddy</t>
+  </si>
+  <si>
+    <t>marketplace-ideabuddy</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/marketplace-ideabuddy/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/EEQR0e</t>
+  </si>
+  <si>
+    <t>EasySpeak</t>
+  </si>
+  <si>
+    <t>easyspeak</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/easyspeak/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/Z60JNW</t>
+  </si>
+  <si>
     <t>New</t>
   </si>
   <si>
-    <t>Clickmoat</t>
-  </si>
-  <si>
-    <t>clickmoat</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/clickmoat/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/APLRWx</t>
-  </si>
-  <si>
-    <t>Writeseed</t>
-  </si>
-  <si>
-    <t>writeseed-ai-content-writer</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/writeseed-ai-content-writer/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/19EZra</t>
-  </si>
-  <si>
-    <t>Quizify</t>
-  </si>
-  <si>
-    <t>quizify</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/quizify/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/Vxo2xa</t>
-  </si>
-  <si>
-    <t>Kvitly</t>
-  </si>
-  <si>
-    <t>kvitly</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/kvitly/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/Z60Y6Q</t>
-  </si>
-  <si>
-    <t>Fox Signals</t>
-  </si>
-  <si>
-    <t>fox-signals</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/fox-signals/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/gOyaOO</t>
-  </si>
-  <si>
-    <t>Bizreply</t>
-  </si>
-  <si>
-    <t>Laxis.ai</t>
-  </si>
-  <si>
-    <t>laxis-ai</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/laxis-ai-prospect-research/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/Xmz2m4</t>
-  </si>
-  <si>
-    <t>Wordplay</t>
-  </si>
-  <si>
-    <t>wordplay</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/wordplay-long-form-ai-writer/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/BnqRnx</t>
-  </si>
-  <si>
-    <t>Headshotly.ai</t>
-  </si>
-  <si>
-    <t>headshotly-ai</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/headshotly-ai/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/bORjOP</t>
-  </si>
-  <si>
-    <t>Power Formulas</t>
-  </si>
-  <si>
-    <t>power-formulas</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/power-formulas/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/3JbmJX</t>
-  </si>
-  <si>
-    <t>No Code Mba</t>
-  </si>
-  <si>
-    <t>no-code-mba-deal</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/no-code-mba-deal/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/dO45Oq</t>
-  </si>
-  <si>
-    <t>Learniverse</t>
-  </si>
-  <si>
-    <t>learniverse</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/learniverse/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/yqG4qv</t>
-  </si>
-  <si>
-    <t>Yazo.ai</t>
-  </si>
-  <si>
-    <t>yazo-ai</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/yazo-ai-content-generator/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/K0ky0A</t>
-  </si>
-  <si>
-    <t>Seopital</t>
-  </si>
-  <si>
-    <t>seopital</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/seopital/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/LKeRKL</t>
-  </si>
-  <si>
-    <t>Image Colorizer</t>
-  </si>
-  <si>
-    <t>imagecolorizer</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/imagecolorizer/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/qzrOzj</t>
-  </si>
-  <si>
-    <t>Viinyx</t>
-  </si>
-  <si>
-    <t>viinyx</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/viinyx/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/xLAzLd</t>
-  </si>
-  <si>
-    <t>Speechactors</t>
-  </si>
-  <si>
-    <t>speechactors</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/speechactors/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/rajJa5</t>
-  </si>
-  <si>
-    <t>Sheetgpt</t>
-  </si>
-  <si>
-    <t>sheetgpt</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/sheetgpt-chatgpt-google-sheets-integration/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/jeKJev</t>
-  </si>
-  <si>
-    <t>Whatsapp Widget</t>
-  </si>
-  <si>
-    <t>marketplace-whatsapp-widget</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/marketplace-whatsapp-widget/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/PO1mOX</t>
-  </si>
-  <si>
-    <t>Equitest</t>
-  </si>
-  <si>
-    <t>equitest</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/marketplace-equitest-online-valuation-platform/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/kOLJOn</t>
-  </si>
-  <si>
-    <t>OnlineCourseHost</t>
-  </si>
-  <si>
-    <t>onlinecoursehost</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/onlinecoursehost/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/GKrRKr</t>
-  </si>
-  <si>
-    <t>CreativeScore</t>
-  </si>
-  <si>
-    <t>creative-score</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/creative-score/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/19EZ9a</t>
-  </si>
-  <si>
-    <t>Airfive</t>
-  </si>
-  <si>
-    <t>airfive</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/airfive/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/Vxo2Oa</t>
-  </si>
-  <si>
-    <t>Bugsmash</t>
-  </si>
-  <si>
-    <t>bugsmash</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/bugsmash/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/JK5Rkr</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/reoon-email-verifier/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/Z60YVQ</t>
-  </si>
-  <si>
-    <t>Screpy</t>
-  </si>
-  <si>
-    <t>screpy</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/screpy/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/BnqR5x</t>
-  </si>
-  <si>
-    <t>Vocal</t>
-  </si>
-  <si>
-    <t>marketplace-vocal</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/marketplace-vocal/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/zx1nze</t>
-  </si>
-  <si>
-    <t>IdeaBuddy</t>
-  </si>
-  <si>
-    <t>marketplace-ideabuddy</t>
-  </si>
-  <si>
-    <t>https://appsumo.com/products/marketplace-ideabuddy/</t>
-  </si>
-  <si>
-    <t>https://appsumo.8odi.net/EEQR0e</t>
+    <t>GoEmailTracker</t>
+  </si>
+  <si>
+    <t>goemailtracker</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/goemailtracker/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/XmzoNM</t>
+  </si>
+  <si>
+    <t>Interactive Shell</t>
+  </si>
+  <si>
+    <t>interactive-shell</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/interactive-shell/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/BnqeP4</t>
+  </si>
+  <si>
+    <t>CapitalConnector.ai</t>
+  </si>
+  <si>
+    <t>capitalconnectorai</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/capitalconnectorai/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/WyBJNn</t>
+  </si>
+  <si>
+    <t>CodeSmash</t>
+  </si>
+  <si>
+    <t>codesmash</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/codesmash/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/090XPL</t>
+  </si>
+  <si>
+    <t>Feedbeo</t>
+  </si>
+  <si>
+    <t>feedbeo</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/feedbeo/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/nXDjya</t>
+  </si>
+  <si>
+    <t>Tabby</t>
+  </si>
+  <si>
+    <t>tabby</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/tabby/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/6y2XE3</t>
+  </si>
+  <si>
+    <t>Arvow</t>
+  </si>
+  <si>
+    <t>arvow</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/arvow/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/2anXdG</t>
+  </si>
+  <si>
+    <t>Trainwel</t>
+  </si>
+  <si>
+    <t>trainwel</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/trainwel/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/vPe1jN</t>
+  </si>
+  <si>
+    <t>DodgePrint</t>
+  </si>
+  <si>
+    <t>dodge-print</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/dodge-print/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/7a3LOO</t>
+  </si>
+  <si>
+    <t>DijiBot</t>
+  </si>
+  <si>
+    <t>dijibot</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/dijibot/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/QjVznz</t>
+  </si>
+  <si>
+    <t>Better Sheets</t>
+  </si>
+  <si>
+    <t>better-sheets</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/better-sheets/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/jeKDya</t>
+  </si>
+  <si>
+    <t>Smart Spreadsheets</t>
+  </si>
+  <si>
+    <t>smart-spreadsheets</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/smart-spreadsheets/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/55OmZD</t>
+  </si>
+  <si>
+    <t>Sheetany</t>
+  </si>
+  <si>
+    <t>sheetany</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/sheetany/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/aO3YAQ</t>
+  </si>
+  <si>
+    <t>Editor.do</t>
+  </si>
+  <si>
+    <t>editordo</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/editordo/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/19EoPB</t>
+  </si>
+  <si>
+    <t>SlideFill</t>
+  </si>
+  <si>
+    <t>slidefill</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/slidefill/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/VxoRYk</t>
+  </si>
+  <si>
+    <t>Grain</t>
+  </si>
+  <si>
+    <t>grain</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/grain/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/Z60JKW</t>
+  </si>
+  <si>
+    <t>Trebble</t>
+  </si>
+  <si>
+    <t>trebble-online-audio-editor</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/trebble-online-audio-editor/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/XmzonM</t>
+  </si>
+  <si>
+    <t>Clawdia</t>
+  </si>
+  <si>
+    <t>clawdia</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/clawdia/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/WyBJdn</t>
+  </si>
+  <si>
+    <t>Vibeo</t>
+  </si>
+  <si>
+    <t>vibeo</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/vibeo/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/bORvN6</t>
+  </si>
+  <si>
+    <t>Vizologi</t>
+  </si>
+  <si>
+    <t>vizologi-plus-exclusive</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/vizologi-plus-exclusive/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/6y2Xd3</t>
+  </si>
+  <si>
+    <t>Produktly</t>
+  </si>
+  <si>
+    <t>produktly</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/produktly/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/2anX5G</t>
+  </si>
+  <si>
+    <t>kiwilaunch</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/kiwilaunch/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/3JbXoA</t>
+  </si>
+  <si>
+    <t>Open eLMS</t>
+  </si>
+  <si>
+    <t>open-elms</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/open-elms/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/RGJYmy</t>
+  </si>
+  <si>
+    <t>ApproveThis</t>
+  </si>
+  <si>
+    <t>approvethis</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/approvethis/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/dO43ny</t>
+  </si>
+  <si>
+    <t>Columns</t>
+  </si>
+  <si>
+    <t>columns-ai</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/columns-ai/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/7a3LoO</t>
+  </si>
+  <si>
+    <t>Lapsula</t>
+  </si>
+  <si>
+    <t>lapsula</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/lapsula/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/xLAXQO</t>
+  </si>
+  <si>
+    <t>Measuremate</t>
+  </si>
+  <si>
+    <t>measuremate</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/measuremate/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/DyDAnq</t>
+  </si>
+  <si>
+    <t>Picbolt</t>
+  </si>
+  <si>
+    <t>picbolt</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/picbolt/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/9LvxOQ</t>
+  </si>
+  <si>
+    <t>Graficto</t>
+  </si>
+  <si>
+    <t>graficto</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/graficto/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/kOLQZv</t>
+  </si>
+  <si>
+    <t>Mystrika</t>
+  </si>
+  <si>
+    <t>mystrika</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/mystrika/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/xLAXQ3</t>
+  </si>
+  <si>
+    <t>Spokk</t>
+  </si>
+  <si>
+    <t>spokk</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/spokk/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/9LvxOY</t>
+  </si>
+  <si>
+    <t>Support Board</t>
+  </si>
+  <si>
+    <t>support-board</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/support-board/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/55OmYo</t>
+  </si>
+  <si>
+    <t>Social Media Canva</t>
+  </si>
+  <si>
+    <t>social-media-canva</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/social-media-canva-template-bundle/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/APLk2J</t>
+  </si>
+  <si>
+    <t>NativeRest</t>
+  </si>
+  <si>
+    <t>nativerest</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/nativerest/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/JK5o4e</t>
+  </si>
+  <si>
+    <t>RenderCut</t>
+  </si>
+  <si>
+    <t>rendercut</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/rendercut/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/Z60JB0</t>
+  </si>
+  <si>
+    <t>Pin Generator</t>
+  </si>
+  <si>
+    <t>pin-generator</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/pin-generator-automated-pinterest-marketing/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/gOyLgv</t>
+  </si>
+  <si>
+    <t>NodeLand</t>
+  </si>
+  <si>
+    <t>cmaps</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/cmaps/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/RGJYZ2</t>
+  </si>
+  <si>
+    <t>WP Login Lockdown</t>
+  </si>
+  <si>
+    <t>wp-login-lockdown</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/wp-login-lockdown/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/4G6RyL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTILA </t>
+  </si>
+  <si>
+    <t>marketplace-rtila</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/marketplace-rtila-growth-hacking-marketing-automation-software/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/yqGEjB</t>
+  </si>
+  <si>
+    <t>nichesss</t>
+  </si>
+  <si>
+    <t>marketplace-nichesss</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/marketplace-nichesss/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/YRW4bK</t>
+  </si>
+  <si>
+    <t>ProxiedMail</t>
+  </si>
+  <si>
+    <t>proxiedmail</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/proxiedmail/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/K0k2Ov</t>
+  </si>
+  <si>
+    <t>Local Rank Tracker</t>
+  </si>
+  <si>
+    <t>local-rank-tracker</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/local-rank-tracker/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/7a3LnV</t>
+  </si>
+  <si>
+    <t>CutMe Short</t>
+  </si>
+  <si>
+    <t>cutme-short</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/cutme-short/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/LKeoO3</t>
+  </si>
+  <si>
+    <t>Img.Upscaler</t>
+  </si>
+  <si>
+    <t>imgupscaler</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/imgupscaler/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/9LvxnY</t>
+  </si>
+  <si>
+    <t>AnyChat</t>
+  </si>
+  <si>
+    <t>anychat</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/anychat/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/19Eoy6</t>
+  </si>
+  <si>
+    <t>Sterling Stock Picker</t>
+  </si>
+  <si>
+    <t>sterling-stock-picker</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/sterling-stock-picker/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/gOyLqv</t>
+  </si>
+  <si>
+    <t>More Good Reviews</t>
+  </si>
+  <si>
+    <t>more-good-reviews</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/more-good-reviews/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/BnqeR0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPDF - PDF Editor </t>
+  </si>
+  <si>
+    <t>updf</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/updf/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/WyBJ2O</t>
+  </si>
+  <si>
+    <t>Stackby</t>
+  </si>
+  <si>
+    <t>stackby</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/stackby/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/vPe1EW</t>
+  </si>
+  <si>
+    <t>Wiz Write</t>
+  </si>
+  <si>
+    <t>wiz-write</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/wiz-write/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/9LvxyY</t>
+  </si>
+  <si>
+    <t>Writecream</t>
+  </si>
+  <si>
+    <t>marketplace-writecream</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/marketplace-writecream/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/jeKDJb</t>
+  </si>
+  <si>
+    <t>NoCodeBackend</t>
+  </si>
+  <si>
+    <t>nocodebackend</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/nocodebackend/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/e1dJk6</t>
+  </si>
+  <si>
+    <t>Deftform</t>
+  </si>
+  <si>
+    <t>deftform</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/deftform/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/9Lvxy4</t>
+  </si>
+  <si>
+    <t>Subpage</t>
+  </si>
+  <si>
+    <t>subpage-deal</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/subpage-deal/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/PO1YBj</t>
+  </si>
+  <si>
+    <t>MetaSurvey</t>
+  </si>
+  <si>
+    <t>products/metasurvey</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/metasurvey/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/Z60JqK</t>
+  </si>
+  <si>
+    <t>FlowyTeam</t>
+  </si>
+  <si>
+    <t>marketplace-flowyteam</t>
+  </si>
+  <si>
+    <t>https://appsumo.com/products/marketplace-flowyteam/</t>
+  </si>
+  <si>
+    <t>https://appsumo.8odi.net/o4QPVo</t>
   </si>
 </sst>
 </file>
@@ -1568,7 +2249,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1769234578" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1769355031" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -1590,7 +2271,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1769234578" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1769355031" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1612,7 +2293,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1769234578"/>
+          <pm:border xmlns:pm="smNativeData" id="1769355031"/>
         </ext>
       </extLst>
     </border>
@@ -1631,7 +2312,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1769234578"/>
+          <pm:border xmlns:pm="smNativeData" id="1769355031"/>
         </ext>
       </extLst>
     </border>
@@ -1639,8 +2320,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -1648,7 +2332,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1769234578" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1769355031" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -1912,16 +2596,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <dimension ref="A1:E128"/>
+  <dimension ref="A1:E185"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="A184" sqref="A184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
   <cols>
     <col min="1" max="1" width="20.378378" customWidth="1" style="0"/>
-    <col min="2" max="2" width="19.081081" customWidth="1" style="0"/>
+    <col min="2" max="2" width="46.000000" customWidth="1" style="0"/>
     <col min="3" max="3" width="48.918919" customWidth="1" style="0"/>
     <col min="4" max="4" width="42.756757" customWidth="1" style="0"/>
     <col min="5" max="5" width="10.000000" style="0"/>
@@ -3624,97 +4308,97 @@
         <v>398</v>
       </c>
       <c r="E100" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" t="s">
+        <v>399</v>
+      </c>
+      <c r="B101" t="s">
         <v>400</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C101" t="s">
         <v>401</v>
       </c>
-      <c r="C101" t="s">
+      <c r="D101" t="s">
         <v>402</v>
       </c>
-      <c r="D101" t="s">
-        <v>403</v>
-      </c>
       <c r="E101" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" t="s">
+        <v>403</v>
+      </c>
+      <c r="B102" t="s">
         <v>404</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" t="s">
         <v>405</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D102" t="s">
         <v>406</v>
       </c>
-      <c r="D102" t="s">
-        <v>407</v>
-      </c>
       <c r="E102" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="A103" t="s">
+        <v>407</v>
+      </c>
+      <c r="B103" t="s">
         <v>408</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C103" t="s">
         <v>409</v>
       </c>
-      <c r="C103" t="s">
+      <c r="D103" t="s">
         <v>410</v>
       </c>
-      <c r="D103" t="s">
-        <v>411</v>
-      </c>
       <c r="E103" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:5">
       <c r="A104" t="s">
+        <v>411</v>
+      </c>
+      <c r="B104" t="s">
         <v>412</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C104" t="s">
         <v>413</v>
       </c>
-      <c r="C104" t="s">
+      <c r="D104" t="s">
         <v>414</v>
       </c>
-      <c r="D104" t="s">
-        <v>415</v>
-      </c>
       <c r="E104" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105" spans="1:5">
       <c r="A105" t="s">
+        <v>415</v>
+      </c>
+      <c r="B105" t="s">
         <v>416</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" t="s">
         <v>417</v>
       </c>
-      <c r="C105" t="s">
+      <c r="D105" t="s">
         <v>418</v>
       </c>
-      <c r="D105" t="s">
-        <v>419</v>
-      </c>
       <c r="E105" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106" spans="1:5">
       <c r="A106" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B106" t="s">
         <v>57</v>
@@ -3726,313 +4410,313 @@
         <v>59</v>
       </c>
       <c r="E106" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="107" spans="1:5">
       <c r="A107" t="s">
+        <v>420</v>
+      </c>
+      <c r="B107" t="s">
         <v>421</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
         <v>422</v>
       </c>
-      <c r="C107" t="s">
+      <c r="D107" t="s">
         <v>423</v>
       </c>
-      <c r="D107" t="s">
-        <v>424</v>
-      </c>
       <c r="E107" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="A108" t="s">
+        <v>424</v>
+      </c>
+      <c r="B108" t="s">
         <v>425</v>
       </c>
-      <c r="B108" t="s">
+      <c r="C108" t="s">
         <v>426</v>
       </c>
-      <c r="C108" t="s">
+      <c r="D108" t="s">
         <v>427</v>
       </c>
-      <c r="D108" t="s">
-        <v>428</v>
-      </c>
       <c r="E108" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="A109" t="s">
+        <v>428</v>
+      </c>
+      <c r="B109" t="s">
         <v>429</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" t="s">
         <v>430</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D109" t="s">
         <v>431</v>
       </c>
-      <c r="D109" t="s">
-        <v>432</v>
-      </c>
       <c r="E109" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" t="s">
+        <v>432</v>
+      </c>
+      <c r="B110" t="s">
         <v>433</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C110" t="s">
         <v>434</v>
       </c>
-      <c r="C110" t="s">
+      <c r="D110" t="s">
         <v>435</v>
       </c>
-      <c r="D110" t="s">
-        <v>436</v>
-      </c>
       <c r="E110" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" t="s">
+        <v>436</v>
+      </c>
+      <c r="B111" t="s">
         <v>437</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" t="s">
         <v>438</v>
       </c>
-      <c r="C111" t="s">
+      <c r="D111" t="s">
         <v>439</v>
       </c>
-      <c r="D111" t="s">
-        <v>440</v>
-      </c>
       <c r="E111" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" t="s">
+        <v>440</v>
+      </c>
+      <c r="B112" t="s">
         <v>441</v>
       </c>
-      <c r="B112" t="s">
+      <c r="C112" t="s">
         <v>442</v>
       </c>
-      <c r="C112" t="s">
+      <c r="D112" t="s">
         <v>443</v>
       </c>
-      <c r="D112" t="s">
-        <v>444</v>
-      </c>
       <c r="E112" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" t="s">
+        <v>444</v>
+      </c>
+      <c r="B113" t="s">
         <v>445</v>
       </c>
-      <c r="B113" t="s">
+      <c r="C113" t="s">
         <v>446</v>
       </c>
-      <c r="C113" t="s">
+      <c r="D113" t="s">
         <v>447</v>
       </c>
-      <c r="D113" t="s">
-        <v>448</v>
-      </c>
       <c r="E113" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" t="s">
+        <v>448</v>
+      </c>
+      <c r="B114" t="s">
         <v>449</v>
       </c>
-      <c r="B114" t="s">
+      <c r="C114" t="s">
         <v>450</v>
       </c>
-      <c r="C114" t="s">
+      <c r="D114" t="s">
         <v>451</v>
       </c>
-      <c r="D114" t="s">
-        <v>452</v>
-      </c>
       <c r="E114" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" t="s">
+        <v>452</v>
+      </c>
+      <c r="B115" t="s">
         <v>453</v>
       </c>
-      <c r="B115" t="s">
+      <c r="C115" t="s">
         <v>454</v>
       </c>
-      <c r="C115" t="s">
+      <c r="D115" t="s">
         <v>455</v>
       </c>
-      <c r="D115" t="s">
-        <v>456</v>
-      </c>
       <c r="E115" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" t="s">
+        <v>456</v>
+      </c>
+      <c r="B116" t="s">
         <v>457</v>
       </c>
-      <c r="B116" t="s">
+      <c r="C116" t="s">
         <v>458</v>
       </c>
-      <c r="C116" t="s">
+      <c r="D116" t="s">
         <v>459</v>
       </c>
-      <c r="D116" t="s">
-        <v>460</v>
-      </c>
       <c r="E116" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" t="s">
+        <v>460</v>
+      </c>
+      <c r="B117" t="s">
         <v>461</v>
       </c>
-      <c r="B117" t="s">
+      <c r="C117" t="s">
         <v>462</v>
       </c>
-      <c r="C117" t="s">
+      <c r="D117" t="s">
         <v>463</v>
       </c>
-      <c r="D117" t="s">
-        <v>464</v>
-      </c>
       <c r="E117" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="118" spans="1:5">
       <c r="A118" t="s">
+        <v>464</v>
+      </c>
+      <c r="B118" t="s">
         <v>465</v>
       </c>
-      <c r="B118" t="s">
+      <c r="C118" t="s">
         <v>466</v>
       </c>
-      <c r="C118" t="s">
+      <c r="D118" t="s">
         <v>467</v>
       </c>
-      <c r="D118" t="s">
-        <v>468</v>
-      </c>
       <c r="E118" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="119" spans="1:5">
       <c r="A119" t="s">
+        <v>468</v>
+      </c>
+      <c r="B119" t="s">
         <v>469</v>
       </c>
-      <c r="B119" t="s">
+      <c r="C119" t="s">
         <v>470</v>
       </c>
-      <c r="C119" t="s">
+      <c r="D119" t="s">
         <v>471</v>
       </c>
-      <c r="D119" t="s">
-        <v>472</v>
-      </c>
       <c r="E119" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:5">
       <c r="A120" t="s">
+        <v>472</v>
+      </c>
+      <c r="B120" t="s">
         <v>473</v>
       </c>
-      <c r="B120" t="s">
+      <c r="C120" t="s">
         <v>474</v>
       </c>
-      <c r="C120" t="s">
+      <c r="D120" t="s">
         <v>475</v>
       </c>
-      <c r="D120" t="s">
-        <v>476</v>
-      </c>
       <c r="E120" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:5">
       <c r="A121" t="s">
+        <v>476</v>
+      </c>
+      <c r="B121" t="s">
         <v>477</v>
       </c>
-      <c r="B121" t="s">
+      <c r="C121" t="s">
         <v>478</v>
       </c>
-      <c r="C121" t="s">
+      <c r="D121" t="s">
         <v>479</v>
       </c>
-      <c r="D121" t="s">
-        <v>480</v>
-      </c>
       <c r="E121" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" t="s">
+        <v>480</v>
+      </c>
+      <c r="B122" t="s">
         <v>481</v>
       </c>
-      <c r="B122" t="s">
+      <c r="C122" t="s">
         <v>482</v>
       </c>
-      <c r="C122" t="s">
+      <c r="D122" t="s">
         <v>483</v>
       </c>
-      <c r="D122" t="s">
-        <v>484</v>
-      </c>
       <c r="E122" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="123" spans="1:5">
       <c r="A123" t="s">
+        <v>484</v>
+      </c>
+      <c r="B123" t="s">
         <v>485</v>
       </c>
-      <c r="B123" t="s">
+      <c r="C123" t="s">
         <v>486</v>
       </c>
-      <c r="C123" t="s">
+      <c r="D123" t="s">
         <v>487</v>
       </c>
-      <c r="D123" t="s">
-        <v>488</v>
-      </c>
       <c r="E123" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="124" spans="1:5">
       <c r="A124" t="s">
+        <v>488</v>
+      </c>
+      <c r="B124" t="s">
         <v>489</v>
       </c>
-      <c r="B124" t="s">
+      <c r="C124" t="s">
         <v>490</v>
       </c>
-      <c r="C124" t="s">
+      <c r="D124" t="s">
         <v>491</v>
       </c>
-      <c r="D124" t="s">
-        <v>492</v>
-      </c>
       <c r="E124" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -4043,71 +4727,1040 @@
         <v>229</v>
       </c>
       <c r="C125" t="s">
+        <v>492</v>
+      </c>
+      <c r="D125" t="s">
         <v>493</v>
       </c>
-      <c r="D125" t="s">
-        <v>494</v>
-      </c>
       <c r="E125" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="126" spans="1:5">
       <c r="A126" t="s">
+        <v>494</v>
+      </c>
+      <c r="B126" t="s">
         <v>495</v>
       </c>
-      <c r="B126" t="s">
+      <c r="C126" t="s">
         <v>496</v>
       </c>
-      <c r="C126" t="s">
+      <c r="D126" t="s">
         <v>497</v>
       </c>
-      <c r="D126" t="s">
-        <v>498</v>
-      </c>
       <c r="E126" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="127" spans="1:5">
       <c r="A127" t="s">
+        <v>498</v>
+      </c>
+      <c r="B127" t="s">
         <v>499</v>
       </c>
-      <c r="B127" t="s">
+      <c r="C127" t="s">
         <v>500</v>
       </c>
-      <c r="C127" t="s">
+      <c r="D127" t="s">
         <v>501</v>
       </c>
-      <c r="D127" t="s">
-        <v>502</v>
-      </c>
       <c r="E127" t="s">
-        <v>399</v>
+        <v>14</v>
       </c>
     </row>
     <row r="128" spans="1:5">
       <c r="A128" t="s">
+        <v>502</v>
+      </c>
+      <c r="B128" t="s">
         <v>503</v>
       </c>
-      <c r="B128" t="s">
+      <c r="C128" t="s">
         <v>504</v>
       </c>
-      <c r="C128" t="s">
+      <c r="D128" t="s">
         <v>505</v>
       </c>
-      <c r="D128" t="s">
+      <c r="E128" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" t="s">
         <v>506</v>
       </c>
-      <c r="E128" t="s">
-        <v>399</v>
+      <c r="B129" t="s">
+        <v>507</v>
+      </c>
+      <c r="C129" t="s">
+        <v>508</v>
+      </c>
+      <c r="D129" t="s">
+        <v>509</v>
+      </c>
+      <c r="E129" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" t="s">
+        <v>511</v>
+      </c>
+      <c r="B130" t="s">
+        <v>512</v>
+      </c>
+      <c r="C130" t="s">
+        <v>513</v>
+      </c>
+      <c r="D130" t="s">
+        <v>514</v>
+      </c>
+      <c r="E130" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" t="s">
+        <v>515</v>
+      </c>
+      <c r="B131" t="s">
+        <v>516</v>
+      </c>
+      <c r="C131" t="s">
+        <v>517</v>
+      </c>
+      <c r="D131" t="s">
+        <v>518</v>
+      </c>
+      <c r="E131" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5">
+      <c r="A132" t="s">
+        <v>519</v>
+      </c>
+      <c r="B132" t="s">
+        <v>520</v>
+      </c>
+      <c r="C132" t="s">
+        <v>521</v>
+      </c>
+      <c r="D132" t="s">
+        <v>522</v>
+      </c>
+      <c r="E132" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133" t="s">
+        <v>523</v>
+      </c>
+      <c r="B133" t="s">
+        <v>524</v>
+      </c>
+      <c r="C133" t="s">
+        <v>525</v>
+      </c>
+      <c r="D133" t="s">
+        <v>526</v>
+      </c>
+      <c r="E133" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
+      <c r="A134" t="s">
+        <v>527</v>
+      </c>
+      <c r="B134" t="s">
+        <v>528</v>
+      </c>
+      <c r="C134" t="s">
+        <v>529</v>
+      </c>
+      <c r="D134" t="s">
+        <v>530</v>
+      </c>
+      <c r="E134" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="A135" t="s">
+        <v>531</v>
+      </c>
+      <c r="B135" t="s">
+        <v>532</v>
+      </c>
+      <c r="C135" t="s">
+        <v>533</v>
+      </c>
+      <c r="D135" t="s">
+        <v>534</v>
+      </c>
+      <c r="E135" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
+      <c r="A136" t="s">
+        <v>535</v>
+      </c>
+      <c r="B136" t="s">
+        <v>536</v>
+      </c>
+      <c r="C136" t="s">
+        <v>537</v>
+      </c>
+      <c r="D136" t="s">
+        <v>538</v>
+      </c>
+      <c r="E136" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
+      <c r="A137" t="s">
+        <v>539</v>
+      </c>
+      <c r="B137" t="s">
+        <v>540</v>
+      </c>
+      <c r="C137" t="s">
+        <v>541</v>
+      </c>
+      <c r="D137" t="s">
+        <v>542</v>
+      </c>
+      <c r="E137" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" t="s">
+        <v>543</v>
+      </c>
+      <c r="B138" t="s">
+        <v>544</v>
+      </c>
+      <c r="C138" t="s">
+        <v>545</v>
+      </c>
+      <c r="D138" t="s">
+        <v>546</v>
+      </c>
+      <c r="E138" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
+      <c r="A139" t="s">
+        <v>547</v>
+      </c>
+      <c r="B139" t="s">
+        <v>548</v>
+      </c>
+      <c r="C139" t="s">
+        <v>549</v>
+      </c>
+      <c r="D139" t="s">
+        <v>550</v>
+      </c>
+      <c r="E139" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140" t="s">
+        <v>551</v>
+      </c>
+      <c r="B140" t="s">
+        <v>552</v>
+      </c>
+      <c r="C140" t="s">
+        <v>553</v>
+      </c>
+      <c r="D140" t="s">
+        <v>554</v>
+      </c>
+      <c r="E140" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141" t="s">
+        <v>555</v>
+      </c>
+      <c r="B141" t="s">
+        <v>556</v>
+      </c>
+      <c r="C141" t="s">
+        <v>557</v>
+      </c>
+      <c r="D141" t="s">
+        <v>558</v>
+      </c>
+      <c r="E141" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142" t="s">
+        <v>559</v>
+      </c>
+      <c r="B142" t="s">
+        <v>560</v>
+      </c>
+      <c r="C142" t="s">
+        <v>561</v>
+      </c>
+      <c r="D142" t="s">
+        <v>562</v>
+      </c>
+      <c r="E142" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143" t="s">
+        <v>563</v>
+      </c>
+      <c r="B143" t="s">
+        <v>564</v>
+      </c>
+      <c r="C143" t="s">
+        <v>565</v>
+      </c>
+      <c r="D143" t="s">
+        <v>566</v>
+      </c>
+      <c r="E143" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
+      <c r="A144" t="s">
+        <v>567</v>
+      </c>
+      <c r="B144" t="s">
+        <v>568</v>
+      </c>
+      <c r="C144" t="s">
+        <v>569</v>
+      </c>
+      <c r="D144" t="s">
+        <v>570</v>
+      </c>
+      <c r="E144" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145" t="s">
+        <v>571</v>
+      </c>
+      <c r="B145" t="s">
+        <v>572</v>
+      </c>
+      <c r="C145" t="s">
+        <v>573</v>
+      </c>
+      <c r="D145" t="s">
+        <v>574</v>
+      </c>
+      <c r="E145" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146" t="s">
+        <v>575</v>
+      </c>
+      <c r="B146" t="s">
+        <v>576</v>
+      </c>
+      <c r="C146" t="s">
+        <v>577</v>
+      </c>
+      <c r="D146" t="s">
+        <v>578</v>
+      </c>
+      <c r="E146" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="A147" t="s">
+        <v>579</v>
+      </c>
+      <c r="B147" t="s">
+        <v>580</v>
+      </c>
+      <c r="C147" t="s">
+        <v>581</v>
+      </c>
+      <c r="D147" t="s">
+        <v>582</v>
+      </c>
+      <c r="E147" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="A148" t="s">
+        <v>583</v>
+      </c>
+      <c r="B148" t="s">
+        <v>584</v>
+      </c>
+      <c r="C148" t="s">
+        <v>585</v>
+      </c>
+      <c r="D148" t="s">
+        <v>586</v>
+      </c>
+      <c r="E148" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
+      <c r="A149" t="s">
+        <v>587</v>
+      </c>
+      <c r="B149" t="s">
+        <v>588</v>
+      </c>
+      <c r="C149" t="s">
+        <v>589</v>
+      </c>
+      <c r="D149" t="s">
+        <v>590</v>
+      </c>
+      <c r="E149" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
+      <c r="A150" t="s">
+        <v>591</v>
+      </c>
+      <c r="B150" t="s">
+        <v>592</v>
+      </c>
+      <c r="C150" t="s">
+        <v>593</v>
+      </c>
+      <c r="D150" t="s">
+        <v>594</v>
+      </c>
+      <c r="E150" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="A151" t="s">
+        <v>595</v>
+      </c>
+      <c r="B151" t="s">
+        <v>595</v>
+      </c>
+      <c r="C151" t="s">
+        <v>596</v>
+      </c>
+      <c r="D151" t="s">
+        <v>597</v>
+      </c>
+      <c r="E151" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
+      <c r="A152" t="s">
+        <v>598</v>
+      </c>
+      <c r="B152" t="s">
+        <v>599</v>
+      </c>
+      <c r="C152" t="s">
+        <v>600</v>
+      </c>
+      <c r="D152" t="s">
+        <v>601</v>
+      </c>
+      <c r="E152" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153" t="s">
+        <v>602</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="C153" t="s">
+        <v>604</v>
+      </c>
+      <c r="D153" t="s">
+        <v>605</v>
+      </c>
+      <c r="E153" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5">
+      <c r="A154" t="s">
+        <v>606</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="C154" t="s">
+        <v>608</v>
+      </c>
+      <c r="D154" t="s">
+        <v>609</v>
+      </c>
+      <c r="E154" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5">
+      <c r="A155" t="s">
+        <v>610</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="C155" t="s">
+        <v>612</v>
+      </c>
+      <c r="D155" t="s">
+        <v>613</v>
+      </c>
+      <c r="E155" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5">
+      <c r="A156" t="s">
+        <v>614</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="C156" t="s">
+        <v>616</v>
+      </c>
+      <c r="D156" t="s">
+        <v>617</v>
+      </c>
+      <c r="E156" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
+      <c r="A157" t="s">
+        <v>618</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="C157" t="s">
+        <v>620</v>
+      </c>
+      <c r="D157" t="s">
+        <v>621</v>
+      </c>
+      <c r="E157" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5">
+      <c r="A158" t="s">
+        <v>622</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="C158" t="s">
+        <v>624</v>
+      </c>
+      <c r="D158" t="s">
+        <v>625</v>
+      </c>
+      <c r="E158" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
+      <c r="A159" t="s">
+        <v>626</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="C159" t="s">
+        <v>628</v>
+      </c>
+      <c r="D159" t="s">
+        <v>629</v>
+      </c>
+      <c r="E159" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5">
+      <c r="A160" t="s">
+        <v>630</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="C160" t="s">
+        <v>632</v>
+      </c>
+      <c r="D160" t="s">
+        <v>633</v>
+      </c>
+      <c r="E160" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
+      <c r="A161" t="s">
+        <v>634</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="C161" t="s">
+        <v>636</v>
+      </c>
+      <c r="D161" t="s">
+        <v>637</v>
+      </c>
+      <c r="E161" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5">
+      <c r="A162" t="s">
+        <v>638</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="C162" t="s">
+        <v>640</v>
+      </c>
+      <c r="D162" t="s">
+        <v>641</v>
+      </c>
+      <c r="E162" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5">
+      <c r="A163" t="s">
+        <v>642</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="C163" t="s">
+        <v>644</v>
+      </c>
+      <c r="D163" t="s">
+        <v>645</v>
+      </c>
+      <c r="E163" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5">
+      <c r="A164" t="s">
+        <v>646</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="C164" t="s">
+        <v>648</v>
+      </c>
+      <c r="D164" t="s">
+        <v>649</v>
+      </c>
+      <c r="E164" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5">
+      <c r="A165" t="s">
+        <v>650</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="C165" t="s">
+        <v>652</v>
+      </c>
+      <c r="D165" t="s">
+        <v>653</v>
+      </c>
+      <c r="E165" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5">
+      <c r="A166" t="s">
+        <v>654</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="C166" t="s">
+        <v>656</v>
+      </c>
+      <c r="D166" t="s">
+        <v>657</v>
+      </c>
+      <c r="E166" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5">
+      <c r="A167" t="s">
+        <v>658</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="C167" t="s">
+        <v>660</v>
+      </c>
+      <c r="D167" t="s">
+        <v>661</v>
+      </c>
+      <c r="E167" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5">
+      <c r="A168" t="s">
+        <v>662</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="C168" t="s">
+        <v>664</v>
+      </c>
+      <c r="D168" t="s">
+        <v>665</v>
+      </c>
+      <c r="E168" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5">
+      <c r="A169" t="s">
+        <v>666</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="C169" t="s">
+        <v>668</v>
+      </c>
+      <c r="D169" t="s">
+        <v>669</v>
+      </c>
+      <c r="E169" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5">
+      <c r="A170" t="s">
+        <v>670</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="C170" t="s">
+        <v>672</v>
+      </c>
+      <c r="D170" t="s">
+        <v>673</v>
+      </c>
+      <c r="E170" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5">
+      <c r="A171" t="s">
+        <v>674</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="C171" t="s">
+        <v>676</v>
+      </c>
+      <c r="D171" t="s">
+        <v>677</v>
+      </c>
+      <c r="E171" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5">
+      <c r="A172" t="s">
+        <v>678</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="C172" t="s">
+        <v>680</v>
+      </c>
+      <c r="D172" t="s">
+        <v>681</v>
+      </c>
+      <c r="E172" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5">
+      <c r="A173" t="s">
+        <v>682</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="C173" t="s">
+        <v>684</v>
+      </c>
+      <c r="D173" t="s">
+        <v>685</v>
+      </c>
+      <c r="E173" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5">
+      <c r="A174" t="s">
+        <v>686</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="C174" t="s">
+        <v>688</v>
+      </c>
+      <c r="D174" t="s">
+        <v>689</v>
+      </c>
+      <c r="E174" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5">
+      <c r="A175" t="s">
+        <v>690</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="C175" t="s">
+        <v>692</v>
+      </c>
+      <c r="D175" t="s">
+        <v>693</v>
+      </c>
+      <c r="E175" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5">
+      <c r="A176" t="s">
+        <v>694</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="C176" t="s">
+        <v>696</v>
+      </c>
+      <c r="D176" t="s">
+        <v>697</v>
+      </c>
+      <c r="E176" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="A177" t="s">
+        <v>698</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="C177" t="s">
+        <v>700</v>
+      </c>
+      <c r="D177" t="s">
+        <v>701</v>
+      </c>
+      <c r="E177" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="A178" t="s">
+        <v>702</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="C178" t="s">
+        <v>704</v>
+      </c>
+      <c r="D178" t="s">
+        <v>705</v>
+      </c>
+      <c r="E178" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5">
+      <c r="A179" t="s">
+        <v>706</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="C179" t="s">
+        <v>708</v>
+      </c>
+      <c r="D179" t="s">
+        <v>709</v>
+      </c>
+      <c r="E179" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="A180" t="s">
+        <v>710</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="C180" t="s">
+        <v>712</v>
+      </c>
+      <c r="D180" t="s">
+        <v>713</v>
+      </c>
+      <c r="E180" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="A181" t="s">
+        <v>714</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="C181" t="s">
+        <v>716</v>
+      </c>
+      <c r="D181" t="s">
+        <v>717</v>
+      </c>
+      <c r="E181" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5">
+      <c r="A182" t="s">
+        <v>718</v>
+      </c>
+      <c r="B182" t="s">
+        <v>719</v>
+      </c>
+      <c r="C182" t="s">
+        <v>720</v>
+      </c>
+      <c r="D182" t="s">
+        <v>721</v>
+      </c>
+      <c r="E182" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5">
+      <c r="A183" t="s">
+        <v>722</v>
+      </c>
+      <c r="B183" t="s">
+        <v>723</v>
+      </c>
+      <c r="C183" t="s">
+        <v>724</v>
+      </c>
+      <c r="D183" t="s">
+        <v>725</v>
+      </c>
+      <c r="E183" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5">
+      <c r="A184" t="s">
+        <v>726</v>
+      </c>
+      <c r="B184" t="s">
+        <v>727</v>
+      </c>
+      <c r="C184" t="s">
+        <v>728</v>
+      </c>
+      <c r="D184" t="s">
+        <v>729</v>
+      </c>
+      <c r="E184" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5">
+      <c r="A185" t="s">
+        <v>730</v>
+      </c>
+      <c r="B185" t="s">
+        <v>731</v>
+      </c>
+      <c r="C185" t="s">
+        <v>732</v>
+      </c>
+      <c r="D185" t="s">
+        <v>733</v>
+      </c>
+      <c r="E185" t="s">
+        <v>510</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1769234578" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1769355031" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -4116,16 +5769,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1769234578" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1769234578" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1769234578" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1769234578" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1769355031" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1769355031" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1769355031" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1769355031" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1769234578" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1769355031" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>